<commit_message>
Login Spotify refactorizado con data desde Excel
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/Data.xlsx
+++ b/src/main/resources/Data/Data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\semillero\Occidente\AutomatizacionOccidente\src\main\resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Semillero_Automatizacion\1ClaseAutomatizacionRefactorizadoExcel\AutomatizacionOccidente\src\main\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03518A1A-C112-44A3-9F92-9C836E094E97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22185" windowHeight="8985"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credenciales" sheetId="2" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Usuario</t>
   </si>
@@ -27,14 +28,17 @@
     <t>Clave</t>
   </si>
   <si>
-    <t>carl@mail.com</t>
+    <t>julieth27f@hotmail.com</t>
+  </si>
+  <si>
+    <t>pi79810859nk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -48,6 +52,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -68,15 +80,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -349,16 +364,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -370,15 +385,18 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1">
-        <v>1234</v>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{83AD2B55-E287-47CA-A764-B84957F1E129}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>